<commit_message>
model update in xls sheet
</commit_message>
<xml_diff>
--- a/ucan_propsed_model_objects.xlsx
+++ b/ucan_propsed_model_objects.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="77">
   <si>
     <t>User</t>
   </si>
@@ -56,34 +56,40 @@
     <t>INT</t>
   </si>
   <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>preferrredLangauge</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>communicationLang</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Autogenerated</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>communicationMode</t>
   </si>
   <si>
     <t>ENUM</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Autogenerated</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>PreferrredMode</t>
+    <t>offline,online</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>PreferredStartTime</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
+    <t>startTime</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
   <si>
     <t>description</t>
@@ -95,88 +101,151 @@
     <t>?</t>
   </si>
   <si>
-    <t>PreferredEndTime</t>
-  </si>
-  <si>
-    <t>followers</t>
+    <t>endTime</t>
+  </si>
+  <si>
+    <t>photopath</t>
   </si>
   <si>
     <t>contact</t>
   </si>
   <si>
+    <t>Preferenceid</t>
+  </si>
+  <si>
     <t>UserTopics</t>
   </si>
   <si>
     <t>Question</t>
   </si>
   <si>
-    <t>TopicHasQuestions</t>
+    <t>QuestionRating</t>
+  </si>
+  <si>
+    <t>topicstatusid</t>
+  </si>
+  <si>
+    <t>questionid</t>
+  </si>
+  <si>
+    <t>qratingid</t>
+  </si>
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>questionText</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>topicid</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>enum(expertise,interested)</t>
+  </si>
+  <si>
+    <t>preferredlanguage</t>
+  </si>
+  <si>
+    <t>vote</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>upvote/downvote</t>
+  </si>
+  <si>
+    <t>preferredTime</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>offline/online</t>
+  </si>
+  <si>
+    <t>open/closed</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>NegotitationMessage</t>
   </si>
   <si>
     <t>questionId</t>
   </si>
   <si>
-    <t>userid</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>questionText</t>
-  </si>
-  <si>
-    <t>topicId</t>
-  </si>
-  <si>
-    <t>topicid</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>status</t>
+    <t>answerid</t>
+  </si>
+  <si>
+    <t>seekerid</t>
+  </si>
+  <si>
+    <t>answerText</t>
+  </si>
+  <si>
+    <t>QuestionTag</t>
+  </si>
+  <si>
+    <t>expertid</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>read/accept/reject</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>tagid</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>notificationid</t>
+  </si>
+  <si>
+    <t>attributeid</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
   <si>
     <t>enum</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>likeCount</t>
-  </si>
-  <si>
-    <t>disLikeCount</t>
-  </si>
-  <si>
-    <t>open/closed</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>commnunicationMode</t>
-  </si>
-  <si>
-    <t>offline/online</t>
-  </si>
-  <si>
-    <t>Negotitation</t>
-  </si>
-  <si>
-    <t>answeId</t>
-  </si>
-  <si>
-    <t>answerText</t>
-  </si>
-  <si>
-    <t>AnswerInfo</t>
-  </si>
-  <si>
-    <t>expertId</t>
+    <t>answer,seekerrequest,requeststatus,discussion</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>read,unread</t>
+  </si>
+  <si>
+    <t>aratingid</t>
   </si>
 </sst>
 </file>
@@ -424,7 +493,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -550,6 +619,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -574,10 +647,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:M33"/>
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L39" activeCellId="0" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -598,7 +671,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -611,7 +684,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
@@ -639,7 +712,7 @@
       </c>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
@@ -669,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="12" t="s">
         <v>13</v>
       </c>
@@ -699,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="12" t="s">
         <v>18</v>
       </c>
@@ -716,9 +789,11 @@
         <v>8</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="K6" s="12" t="s">
         <v>7</v>
       </c>
@@ -729,9 +804,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>8</v>
@@ -740,17 +815,17 @@
         <v>9</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I7" s="14"/>
       <c r="K7" s="12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L7" s="13" t="s">
         <v>8</v>
@@ -759,43 +834,52 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I8" s="23"/>
       <c r="K8" s="20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L8" s="21"/>
       <c r="M8" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>9</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -812,18 +896,18 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3"/>
       <c r="K14" s="1"/>
       <c r="L14" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M14" s="3"/>
     </row>
@@ -858,7 +942,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="24" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>17</v>
@@ -867,7 +951,7 @@
         <v>12</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>17</v>
@@ -876,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="L16" s="13" t="s">
         <v>17</v>
@@ -887,16 +971,16 @@
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>8</v>
@@ -905,27 +989,27 @@
         <v>9</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>8</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>8</v>
@@ -933,25 +1017,40 @@
       <c r="H18" s="14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,56 +1064,56 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G21" s="13"/>
       <c r="H21" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G22" s="13"/>
       <c r="H22" s="14" t="s">
-        <v>12</v>
+        <v>49</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="20" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="K24" s="0" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="G24" s="31"/>
+      <c r="H24" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,18 +1127,16 @@
         <v>4</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>17</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="L25" s="16"/>
       <c r="M25" s="28" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="12" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>17</v>
@@ -1048,18 +1145,16 @@
         <v>12</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L26" s="25" t="s">
-        <v>17</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="L26" s="25"/>
       <c r="M26" s="26" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="12" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>8</v>
@@ -1069,22 +1164,23 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="2" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H27" s="3"/>
       <c r="K27" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>8</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="14" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>2</v>
@@ -1095,22 +1191,22 @@
       <c r="H28" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K28" s="32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>12</v>
-      </c>
+      <c r="K28" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
       <c r="F29" s="12" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>17</v>
@@ -1118,10 +1214,19 @@
       <c r="H29" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="K29" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="15" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>17</v>
@@ -1130,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G30" s="25"/>
       <c r="H30" s="26" t="s">
@@ -1148,7 +1253,7 @@
         <v>12</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>8</v>
@@ -1166,6 +1271,114 @@
       <c r="F33" s="15"/>
       <c r="G33" s="16"/>
       <c r="H33" s="28"/>
+      <c r="K33" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K34" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K35" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1"/>
+      <c r="C36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="K36" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>